<commit_message>
Neue Version - BK
</commit_message>
<xml_diff>
--- a/Schnittstellen Beschreibung/Views from DELTEK.xlsx
+++ b/Schnittstellen Beschreibung/Views from DELTEK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaspe\Documents\ILF\Schnittstellen Beschreibung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6227E6C2-D712-429A-AB00-CF3228FEB031}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C998129F-3F3A-476D-8AA2-EFC126B6E403}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{1B1C8240-F260-46F3-8DA1-CB42D6A8C6D3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="417">
   <si>
     <t>Ressource_Firmencode</t>
   </si>
@@ -526,9 +526,6 @@
     <t>Buchungsperiode</t>
   </si>
   <si>
-    <t>UnterProjektnr</t>
-  </si>
-  <si>
     <t>Arbeitsauftragsnr</t>
   </si>
   <si>
@@ -710,9 +707,6 @@
   </si>
   <si>
     <t>BookingPeriod</t>
-  </si>
-  <si>
-    <t>SubprojectNr</t>
   </si>
   <si>
     <t>MainprojectNr</t>
@@ -1182,9 +1176,6 @@
   </si>
   <si>
     <t>ACTIVITYNUMBER</t>
-  </si>
-  <si>
-    <t>JOBNUMBER</t>
   </si>
   <si>
     <t>JOBNUMBER (kann drauf gebucht werden….)</t>
@@ -1303,6 +1294,12 @@
 ,'PREVIOUSEMPLOYEENUMBER'
 ,'ENTITYNAME'
 )</t>
+  </si>
+  <si>
+    <t>Eintragsnummer</t>
+  </si>
+  <si>
+    <t>Entrynumber</t>
   </si>
 </sst>
 </file>
@@ -4334,9 +4331,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:N239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H220" sqref="H219:H220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4351,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>22</v>
@@ -4363,22 +4360,22 @@
         <v>23</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -4391,7 +4388,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="1"/>
       <c r="I2" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4403,10 +4400,10 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4418,10 +4415,10 @@
       </c>
       <c r="E4" s="7"/>
       <c r="F4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -4436,10 +4433,10 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4451,10 +4448,10 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4466,10 +4463,10 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4481,10 +4478,10 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4496,25 +4493,25 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,7 +4523,7 @@
       </c>
       <c r="E11" s="7"/>
       <c r="I11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4538,15 +4535,15 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>158</v>
@@ -4556,10 +4553,10 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4574,13 +4571,13 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4617,10 +4614,10 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -4632,7 +4629,7 @@
       </c>
       <c r="E19" s="7"/>
       <c r="G19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -4640,14 +4637,14 @@
         <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -4658,14 +4655,14 @@
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G21" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -4673,14 +4670,14 @@
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H22" s="9"/>
     </row>
@@ -4689,14 +4686,14 @@
         <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H23" s="14"/>
     </row>
@@ -4705,17 +4702,17 @@
         <v>30</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -4723,11 +4720,11 @@
         <v>31</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E25" s="7"/>
       <c r="N25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -4735,14 +4732,14 @@
         <v>32</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -4750,14 +4747,14 @@
         <v>33</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -4769,10 +4766,10 @@
       </c>
       <c r="E28" s="7"/>
       <c r="F28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -4780,14 +4777,14 @@
         <v>35</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -4795,14 +4792,14 @@
         <v>36</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G30" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -4810,14 +4807,14 @@
         <v>37</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -4825,14 +4822,14 @@
         <v>38</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -4840,14 +4837,14 @@
         <v>39</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G33" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -4861,17 +4858,17 @@
         <v>41</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G35" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I35" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
@@ -4879,11 +4876,11 @@
         <v>42</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -4891,14 +4888,14 @@
         <v>43</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G37" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -4906,7 +4903,7 @@
         <v>44</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E38" s="7"/>
     </row>
@@ -4915,17 +4912,17 @@
         <v>45</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G39" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
@@ -4933,10 +4930,10 @@
         <v>46</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E40" s="7"/>
     </row>
@@ -4945,17 +4942,17 @@
         <v>47</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D41" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G41" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -4963,10 +4960,10 @@
         <v>48</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E42" s="7"/>
     </row>
@@ -4975,17 +4972,17 @@
         <v>49</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
@@ -4993,10 +4990,10 @@
         <v>50</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E44" s="7"/>
     </row>
@@ -5005,17 +5002,17 @@
         <v>51</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G45" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -5023,10 +5020,10 @@
         <v>52</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E46" s="7"/>
     </row>
@@ -5035,17 +5032,17 @@
         <v>53</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G47" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
@@ -5053,10 +5050,10 @@
         <v>54</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E48" s="7"/>
     </row>
@@ -5065,17 +5062,17 @@
         <v>55</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G49" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -5083,10 +5080,10 @@
         <v>56</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E50" s="7"/>
     </row>
@@ -5095,17 +5092,17 @@
         <v>57</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G51" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -5113,10 +5110,10 @@
         <v>58</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E52" s="7"/>
     </row>
@@ -5125,17 +5122,17 @@
         <v>59</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G53" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -5143,10 +5140,10 @@
         <v>60</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D54" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E54" s="7"/>
     </row>
@@ -5155,17 +5152,17 @@
         <v>61</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G55" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
@@ -5173,10 +5170,10 @@
         <v>62</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D56" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E56" s="7"/>
     </row>
@@ -5185,17 +5182,17 @@
         <v>63</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G57" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -5203,10 +5200,10 @@
         <v>64</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E58" s="7"/>
     </row>
@@ -5215,17 +5212,17 @@
         <v>65</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
@@ -5233,10 +5230,10 @@
         <v>66</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E60" s="7"/>
     </row>
@@ -5245,14 +5242,14 @@
         <v>67</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -5260,18 +5257,18 @@
         <v>68</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H62" s="14"/>
       <c r="I62" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -5279,79 +5276,79 @@
         <v>70</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E68" s="7"/>
       <c r="F68" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H68" s="14"/>
     </row>
@@ -5405,7 +5402,7 @@
       </c>
       <c r="E74" s="7"/>
       <c r="G74" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -5443,7 +5440,7 @@
         <v>158</v>
       </c>
       <c r="D78" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E78" s="7"/>
     </row>
@@ -5455,7 +5452,7 @@
         <v>158</v>
       </c>
       <c r="D79" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E79" s="7"/>
     </row>
@@ -5512,7 +5509,7 @@
         <v>158</v>
       </c>
       <c r="D85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E85" s="7"/>
     </row>
@@ -5524,7 +5521,7 @@
         <v>158</v>
       </c>
       <c r="D86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E86" s="7"/>
     </row>
@@ -5536,7 +5533,7 @@
         <v>158</v>
       </c>
       <c r="D87" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E87" s="7"/>
     </row>
@@ -5548,7 +5545,7 @@
         <v>158</v>
       </c>
       <c r="D88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E88" s="7"/>
     </row>
@@ -5560,7 +5557,7 @@
         <v>158</v>
       </c>
       <c r="D89" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E89" s="7"/>
     </row>
@@ -5572,7 +5569,7 @@
         <v>158</v>
       </c>
       <c r="D90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" s="7"/>
     </row>
@@ -5584,7 +5581,7 @@
         <v>158</v>
       </c>
       <c r="D91" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E91" s="7"/>
     </row>
@@ -5596,7 +5593,7 @@
         <v>158</v>
       </c>
       <c r="D92" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E92" s="7"/>
     </row>
@@ -5608,7 +5605,7 @@
         <v>158</v>
       </c>
       <c r="D93" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E93" s="7"/>
     </row>
@@ -5620,7 +5617,7 @@
         <v>158</v>
       </c>
       <c r="D94" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E94" s="7"/>
     </row>
@@ -5632,7 +5629,7 @@
         <v>158</v>
       </c>
       <c r="D95" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E95" s="7"/>
     </row>
@@ -5644,7 +5641,7 @@
         <v>158</v>
       </c>
       <c r="D96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E96" s="7"/>
     </row>
@@ -5656,7 +5653,7 @@
         <v>158</v>
       </c>
       <c r="D97" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E97" s="7"/>
     </row>
@@ -5668,7 +5665,7 @@
         <v>158</v>
       </c>
       <c r="D98" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E98" s="7"/>
     </row>
@@ -5680,7 +5677,7 @@
         <v>158</v>
       </c>
       <c r="D99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E99" s="7"/>
     </row>
@@ -5692,7 +5689,7 @@
         <v>158</v>
       </c>
       <c r="D100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E100" s="7"/>
     </row>
@@ -5704,7 +5701,7 @@
         <v>158</v>
       </c>
       <c r="D101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E101" s="7"/>
     </row>
@@ -5716,7 +5713,7 @@
         <v>158</v>
       </c>
       <c r="D102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E102" s="7"/>
     </row>
@@ -5728,7 +5725,7 @@
         <v>158</v>
       </c>
       <c r="D103" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E103" s="7"/>
     </row>
@@ -5740,7 +5737,7 @@
         <v>158</v>
       </c>
       <c r="D104" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E104" s="7"/>
     </row>
@@ -5752,7 +5749,7 @@
         <v>158</v>
       </c>
       <c r="D105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E105" s="7"/>
     </row>
@@ -5764,7 +5761,7 @@
         <v>158</v>
       </c>
       <c r="D106" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E106" s="7"/>
     </row>
@@ -5776,7 +5773,7 @@
         <v>158</v>
       </c>
       <c r="D107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E107" s="7"/>
     </row>
@@ -5788,7 +5785,7 @@
         <v>158</v>
       </c>
       <c r="D108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E108" s="7"/>
     </row>
@@ -5809,7 +5806,7 @@
         <v>158</v>
       </c>
       <c r="D110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E110" s="7"/>
     </row>
@@ -5824,44 +5821,44 @@
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E112" s="7"/>
       <c r="F112" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G112" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E113" s="7"/>
       <c r="F113" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G113" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H114" s="14"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E115" s="7"/>
       <c r="G115" s="14"/>
@@ -5869,11 +5866,11 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E116" s="7"/>
       <c r="G116" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H116" s="14"/>
     </row>
@@ -5915,7 +5912,7 @@
       </c>
       <c r="E121" s="7"/>
       <c r="F121" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5945,7 +5942,7 @@
       </c>
       <c r="E124" s="7"/>
       <c r="G124" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -5953,11 +5950,11 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E125" s="7"/>
       <c r="G125" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -5972,7 +5969,7 @@
       </c>
       <c r="E126" s="7"/>
       <c r="G126" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5995,11 +5992,11 @@
         <v>158</v>
       </c>
       <c r="D128" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E128" s="7"/>
       <c r="G128" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -6010,7 +6007,7 @@
         <v>158</v>
       </c>
       <c r="D129" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E129" s="7"/>
     </row>
@@ -6039,10 +6036,13 @@
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>148</v>
+      </c>
+      <c r="H133">
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -6055,7 +6055,7 @@
       <c r="E134" s="7"/>
       <c r="F134" s="4"/>
       <c r="G134" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H134" s="2"/>
     </row>
@@ -6069,7 +6069,7 @@
       <c r="E135" s="7"/>
       <c r="F135" s="4"/>
       <c r="G135" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -6106,11 +6106,11 @@
         <v>158</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F138" s="15"/>
       <c r="I138" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6121,11 +6121,11 @@
         <v>158</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F139" s="15"/>
       <c r="I139" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -6140,7 +6140,6 @@
       <c r="G140" t="s">
         <v>153</v>
       </c>
-      <c r="H140" s="9"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
@@ -6165,7 +6164,7 @@
       <c r="E142" s="7"/>
       <c r="F142" s="4"/>
       <c r="G142" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -6178,7 +6177,7 @@
       <c r="E143" s="7"/>
       <c r="F143" s="4"/>
       <c r="G143" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6186,12 +6185,11 @@
         <v>147</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F144" s="15"/>
-      <c r="H144"/>
       <c r="I144" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -6203,7 +6201,6 @@
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="4"/>
-      <c r="H145" s="9"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E146" s="7"/>
@@ -6227,10 +6224,10 @@
       </c>
       <c r="E148" s="7"/>
       <c r="F148" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G148" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -6242,7 +6239,7 @@
       </c>
       <c r="E149" s="7"/>
       <c r="G149" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -6254,7 +6251,7 @@
       </c>
       <c r="E150" s="7"/>
       <c r="G150" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -6277,7 +6274,7 @@
     </row>
     <row r="154" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -6287,301 +6284,270 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>371</v>
-      </c>
-      <c r="C155" t="s">
-        <v>158</v>
+        <v>369</v>
       </c>
       <c r="D155" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E155" s="7"/>
       <c r="F155" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G155" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>372</v>
-      </c>
-      <c r="C156" t="s">
-        <v>158</v>
+        <v>370</v>
       </c>
       <c r="D156" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E156" s="7"/>
       <c r="F156" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G156" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>136</v>
       </c>
-      <c r="C157" t="s">
-        <v>158</v>
-      </c>
       <c r="D157" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E157" s="7"/>
       <c r="F157" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G157" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>166</v>
-      </c>
-      <c r="C158" t="s">
-        <v>158</v>
+        <v>25</v>
       </c>
       <c r="D158" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E158" s="7"/>
       <c r="F158" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G158" t="s">
-        <v>385</v>
+        <v>383</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>25</v>
-      </c>
-      <c r="C159" t="s">
-        <v>158</v>
+        <v>415</v>
       </c>
       <c r="D159" t="s">
-        <v>229</v>
+        <v>416</v>
       </c>
       <c r="E159" s="7"/>
-      <c r="F159" t="s">
-        <v>350</v>
-      </c>
       <c r="G159" t="s">
-        <v>386</v>
+        <v>416</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>1</v>
       </c>
-      <c r="C160" t="s">
-        <v>158</v>
-      </c>
       <c r="D160" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E160" s="7"/>
       <c r="F160" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G160" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="161" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>167</v>
-      </c>
-      <c r="C161" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D161" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E161" s="7"/>
       <c r="F161" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G161" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="162" spans="2:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C162" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="D162" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="H162"/>
+        <v>226</v>
+      </c>
     </row>
     <row r="163" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>168</v>
-      </c>
-      <c r="C163" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D163" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E163" s="7"/>
       <c r="F163" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G163" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="164" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>169</v>
-      </c>
-      <c r="C164" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D164" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E164" s="7"/>
       <c r="F164" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G164" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="165" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E165" s="7"/>
       <c r="F165" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G165" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="166" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E166" s="7"/>
       <c r="F166" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G166" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="167" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E167" s="7"/>
       <c r="F167" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G167" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="168" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="C168" s="14" t="s">
-        <v>158</v>
+        <v>349</v>
       </c>
       <c r="D168" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E168" s="7"/>
       <c r="F168" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G168" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H168"/>
     </row>
     <row r="169" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D169" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E169" s="7"/>
       <c r="F169" t="s">
+        <v>352</v>
+      </c>
+      <c r="G169" t="s">
         <v>354</v>
-      </c>
-      <c r="G169" t="s">
-        <v>356</v>
       </c>
       <c r="H169" s="14"/>
     </row>
     <row r="170" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D170" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E170" s="7"/>
       <c r="F170" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G170" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="171" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D171" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E171" s="7"/>
       <c r="F171" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G171" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="172" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E172" s="7"/>
       <c r="F172" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G172" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="173" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E173" s="7"/>
       <c r="F173" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G173" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="174" spans="2:8" x14ac:dyDescent="0.25">
@@ -6591,17 +6557,14 @@
       <c r="B175" t="s">
         <v>11</v>
       </c>
-      <c r="C175" t="s">
-        <v>158</v>
-      </c>
       <c r="D175" t="s">
         <v>11</v>
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="177" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -6609,60 +6572,66 @@
       <c r="E177" s="7"/>
       <c r="F177" s="1"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
+        <v>307</v>
+      </c>
+      <c r="F178" t="s">
+        <v>312</v>
+      </c>
+      <c r="G178" t="s">
+        <v>307</v>
+      </c>
+      <c r="H178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>306</v>
+      </c>
+      <c r="G179" t="s">
+        <v>306</v>
+      </c>
+      <c r="H179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>308</v>
+      </c>
+      <c r="G180" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
         <v>309</v>
       </c>
-      <c r="F178" t="s">
-        <v>314</v>
-      </c>
-      <c r="G178" t="s">
+      <c r="G181" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>308</v>
-      </c>
-      <c r="G179" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B180" t="s">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
         <v>310</v>
       </c>
-      <c r="G180" t="s">
+      <c r="G182" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>311</v>
-      </c>
-      <c r="G181" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B182" t="s">
-        <v>312</v>
-      </c>
-      <c r="G182" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G183" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -6670,22 +6639,25 @@
       <c r="E186" s="7"/>
       <c r="F186" s="1"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F187" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G187" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+      <c r="H187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G188" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -6693,32 +6665,35 @@
       <c r="E190" s="7"/>
       <c r="F190" s="1"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F191" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G191" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+      <c r="H191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G192" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G193" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G194" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -6726,72 +6701,78 @@
       <c r="E195" s="7"/>
       <c r="F195" s="1"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G196" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+      <c r="H196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G197" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="H197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G198" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G199" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G200" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G201" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G202" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G201" t="s">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G203" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G202" t="s">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G204" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G203" t="s">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G205" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G204" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G205" t="s">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G206" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G206" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G207" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -6799,42 +6780,45 @@
       <c r="E210" s="7"/>
       <c r="F210" s="1"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F211" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G211" t="s">
+        <v>400</v>
+      </c>
+      <c r="H211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G212" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G213" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G212" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G213" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G214" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G215" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G216" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="218" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -6842,92 +6826,98 @@
       <c r="E218" s="7"/>
       <c r="F218" s="1"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F219" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G219" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="H219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G220" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="H220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G221" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G222" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G223" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G224" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G225" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G226" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G227" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G228" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G229" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G230" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G231" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G224" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G225" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G226" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G227" t="s">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G232" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G228" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G229" t="s">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G233" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G230" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G231" t="s">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G234" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G232" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G233" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G234" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="236" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -6935,22 +6925,25 @@
       <c r="E236" s="7"/>
       <c r="F236" s="1"/>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F237" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G237" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="H237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G238" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G239" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>